<commit_message>
finalised phonetic figures for phonetic analysis of word boundary
</commit_message>
<xml_diff>
--- a/Ch_6_Form/AH Corpus Foot Ana Word Graphs.xlsx
+++ b/Ch_6_Form/AH Corpus Foot Ana Word Graphs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\antoi\GitHub\PhD\Ch_6_Form\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B8AF1E3-FF89-4A75-9752-3022769DD5E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC56A31-3D50-48FF-8948-2AC099B1349A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{1ABE4724-14B1-4801-819D-892587CA02C5}"/>
   </bookViews>
@@ -488,36 +488,6 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -580,6 +550,36 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="19" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -773,8 +773,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFC8D62"/>
+      <color rgb="FFD95F02"/>
       <color rgb="FF1B9E77"/>
-      <color rgb="FFD95F02"/>
       <color rgb="FF47298A"/>
       <color rgb="FF7570B3"/>
       <color rgb="FFE7298A"/>
@@ -33700,144 +33701,6 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'PN Word Boundaries'!$A$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Lally’s is in-</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>'PN Word Boundaries'!$E$1:$H$1</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>'PN Word Boundaries'!$F$1:$H$1</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>(*)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>L*H</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>&gt;H*</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>H*</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>'PN Word Boundaries'!$E$4:$H$4</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>'PN Word Boundaries'!$F$4:$H$4</c:f>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-DD1C-4CB6-AFDE-41B17C2430C4}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'PN Word Boundaries'!$A$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Valerie’s is</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>'PN Word Boundaries'!$E$1:$H$1</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>'PN Word Boundaries'!$F$1:$H$1</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>(*)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>L*H</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>&gt;H*</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>H*</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>'PN Word Boundaries'!$E$5:$H$5</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>'PN Word Boundaries'!$F$5:$H$5</c:f>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-DD1C-4CB6-AFDE-41B17C2430C4}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
           <c:idx val="4"/>
           <c:order val="4"/>
           <c:tx>
@@ -34121,6 +33984,1392 @@
         <c:overlap val="-27"/>
         <c:axId val="1889305647"/>
         <c:axId val="1889284847"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'PN Word Boundaries'!$A$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Lally’s is in-</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:srgbClr val="D95F02"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:sysClr val="windowText" lastClr="000000"/>
+                          </a:solidFill>
+                          <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="outEnd"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:round/>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>'PN Word Boundaries'!$E$1:$H$1</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>'PN Word Boundaries'!$F$1:$H$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="3"/>
+                      <c:pt idx="0">
+                        <c:v>L*H</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>&gt;H*</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>H*</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>'PN Word Boundaries'!$E$4:$H$4</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>'PN Word Boundaries'!$F$4:$H$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="3"/>
+                      <c:pt idx="0">
+                        <c:v>48</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>3</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000002-DD1C-4CB6-AFDE-41B17C2430C4}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="3"/>
+                <c:order val="3"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'PN Word Boundaries'!$A$5</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Valerie’s is</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:srgbClr val="FC8D62"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>'PN Word Boundaries'!$E$1:$H$1</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>'PN Word Boundaries'!$F$1:$H$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="3"/>
+                      <c:pt idx="0">
+                        <c:v>L*H</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>&gt;H*</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>H*</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>'PN Word Boundaries'!$E$5:$H$5</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>'PN Word Boundaries'!$F$5:$H$5</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="3"/>
+                      <c:pt idx="0">
+                        <c:v>35</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000003-DD1C-4CB6-AFDE-41B17C2430C4}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1889305647"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1889284847"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1889284847"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>count</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1889305647"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="tr"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.72847922134733156"/>
+          <c:y val="0.18287037037037041"/>
+          <c:w val="0.20207633420822393"/>
+          <c:h val="0.31598571011956839"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg2">
+              <a:lumMod val="90000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1000">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart46.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-IE" sz="1000"/>
+              <a:t>Prenuclear pitch</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-IE" sz="1000" baseline="0"/>
+              <a:t> accent counts per target phrase</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-IE" sz="1000"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'PN Word Boundaries'!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Lally’s is</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="8DA0CB"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'PN Word Boundaries'!$E$1:$H$1</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'PN Word Boundaries'!$F$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>L*H</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>&gt;H*</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>H*</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'PN Word Boundaries'!$E$3:$H$3</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'PN Word Boundaries'!$F$3:$H$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9688-4847-BEB1-DE5B257B3296}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'PN Word Boundaries'!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Lally’s is in-</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="D95F02"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'PN Word Boundaries'!$E$1:$H$1</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'PN Word Boundaries'!$F$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>L*H</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>&gt;H*</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>H*</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'PN Word Boundaries'!$E$4:$H$4</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'PN Word Boundaries'!$F$4:$H$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-9688-4847-BEB1-DE5B257B3296}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1889305647"/>
+        <c:axId val="1889284847"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'PN Word Boundaries'!$A$2</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Val’s is in-</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:srgbClr val="7570B3"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:sysClr val="windowText" lastClr="000000"/>
+                          </a:solidFill>
+                          <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="outEnd"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:round/>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>'PN Word Boundaries'!$E$1:$H$1</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>'PN Word Boundaries'!$F$1:$H$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="3"/>
+                      <c:pt idx="0">
+                        <c:v>L*H</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>&gt;H*</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>H*</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>'PN Word Boundaries'!$E$2:$H$2</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>'PN Word Boundaries'!$F$2:$H$2</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="3"/>
+                      <c:pt idx="0">
+                        <c:v>35</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>13</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-9688-4847-BEB1-DE5B257B3296}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="3"/>
+                <c:order val="3"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'PN Word Boundaries'!$A$5</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Valerie’s is</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:srgbClr val="FC8D62"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>'PN Word Boundaries'!$E$1:$H$1</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>'PN Word Boundaries'!$F$1:$H$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="3"/>
+                      <c:pt idx="0">
+                        <c:v>L*H</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>&gt;H*</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>H*</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>'PN Word Boundaries'!$E$5:$H$5</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>'PN Word Boundaries'!$F$5:$H$5</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="3"/>
+                      <c:pt idx="0">
+                        <c:v>35</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000003-9688-4847-BEB1-DE5B257B3296}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="4"/>
+                <c:order val="4"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'PN Word Boundaries'!$A$6</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Elaine was a</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:srgbClr val="1B9E77"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:sysClr val="windowText" lastClr="000000"/>
+                          </a:solidFill>
+                          <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="outEnd"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:round/>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>'PN Word Boundaries'!$E$1:$H$1</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>'PN Word Boundaries'!$F$1:$H$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="3"/>
+                      <c:pt idx="0">
+                        <c:v>L*H</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>&gt;H*</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>H*</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>'PN Word Boundaries'!$E$6:$H$6</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>'PN Word Boundaries'!$F$6:$H$6</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="3"/>
+                      <c:pt idx="0">
+                        <c:v>35</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>18</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000004-9688-4847-BEB1-DE5B257B3296}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="5"/>
+                <c:order val="5"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'PN Word Boundaries'!$A$7</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Elaina’s a</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:srgbClr val="66C2A5"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:sysClr val="windowText" lastClr="000000"/>
+                          </a:solidFill>
+                          <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="outEnd"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:round/>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>'PN Word Boundaries'!$E$1:$H$1</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>'PN Word Boundaries'!$F$1:$H$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="3"/>
+                      <c:pt idx="0">
+                        <c:v>L*H</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>&gt;H*</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>H*</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>'PN Word Boundaries'!$E$7:$H$7</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>'PN Word Boundaries'!$F$7:$H$7</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="3"/>
+                      <c:pt idx="0">
+                        <c:v>51</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>4</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000005-9688-4847-BEB1-DE5B257B3296}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
       </c:barChart>
       <c:catAx>
         <c:axId val="1889305647"/>
@@ -39712,6 +40961,46 @@
 </file>
 
 <file path=xl/charts/colors17.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors18.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -44112,6 +45401,509 @@
 </file>
 
 <file path=xl/charts/style17.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style18.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -50440,6 +52232,44 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>16565</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6F24725-5A9A-490D-B4DA-A010C35A897E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -55230,10 +57060,10 @@
         <f t="shared" ref="F2:F5" si="0">B2-C2</f>
         <v>1.7501581088798703</v>
       </c>
-      <c r="R2" s="16" t="s">
+      <c r="R2" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="S2" s="17"/>
+      <c r="S2" s="38"/>
       <c r="T2" s="15"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -55261,10 +57091,10 @@
         <f t="shared" si="0"/>
         <v>2.9959258498736796</v>
       </c>
-      <c r="R3" s="18" t="s">
+      <c r="R3" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="S3" s="19"/>
+      <c r="S3" s="40"/>
       <c r="T3" s="15"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -57075,10 +58905,10 @@
         <f>B2-C2</f>
         <v>7.6542019279553797</v>
       </c>
-      <c r="R2" s="16" t="s">
+      <c r="R2" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="S2" s="17"/>
+      <c r="S2" s="38"/>
       <c r="T2" s="15"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -57106,10 +58936,10 @@
         <f t="shared" ref="F3:F5" si="0">B3-C3</f>
         <v>7.8240381452207099</v>
       </c>
-      <c r="R3" s="18" t="s">
+      <c r="R3" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="S3" s="19"/>
+      <c r="S3" s="40"/>
       <c r="T3" s="15"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -57613,7 +59443,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -57623,228 +59453,228 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="45" t="s">
+      <c r="E1" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="F1" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="G1" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="45" t="s">
+      <c r="H1" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="I1" s="45" t="s">
+      <c r="I1" s="35" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="30">
+      <c r="B2" s="20">
         <v>1</v>
       </c>
-      <c r="C2" s="30">
+      <c r="C2" s="20">
         <v>0</v>
       </c>
-      <c r="D2" s="30">
+      <c r="D2" s="20">
         <v>1</v>
       </c>
-      <c r="E2" s="36">
+      <c r="E2" s="26">
         <v>1</v>
       </c>
-      <c r="F2" s="44">
+      <c r="F2" s="34">
         <v>35</v>
       </c>
-      <c r="G2" s="43">
+      <c r="G2" s="33">
         <v>6</v>
       </c>
-      <c r="H2" s="42">
+      <c r="H2" s="32">
         <v>13</v>
       </c>
-      <c r="I2" s="41">
+      <c r="I2" s="31">
         <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="30">
+      <c r="B3" s="20">
         <v>1</v>
       </c>
-      <c r="C3" s="30">
+      <c r="C3" s="20">
         <v>0</v>
       </c>
-      <c r="D3" s="30">
+      <c r="D3" s="20">
         <v>2</v>
       </c>
-      <c r="E3" s="28">
+      <c r="E3" s="18">
         <v>1</v>
       </c>
-      <c r="F3" s="40">
+      <c r="F3" s="30">
         <v>46</v>
       </c>
-      <c r="G3" s="39">
+      <c r="G3" s="29">
         <v>5</v>
       </c>
-      <c r="H3" s="27">
+      <c r="H3" s="17">
         <v>4</v>
       </c>
-      <c r="I3" s="32">
+      <c r="I3" s="22">
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="31" t="s">
+    <row r="4" spans="1:9" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="30">
+      <c r="B4" s="20">
         <v>2</v>
       </c>
-      <c r="C4" s="30">
+      <c r="C4" s="20">
         <v>0</v>
       </c>
-      <c r="D4" s="30">
+      <c r="D4" s="20">
         <v>2</v>
       </c>
-      <c r="E4" s="37">
+      <c r="E4" s="27">
         <v>3</v>
       </c>
-      <c r="F4" s="38">
+      <c r="F4" s="28">
         <v>48</v>
       </c>
-      <c r="G4" s="34">
+      <c r="G4" s="24">
         <v>2</v>
       </c>
-      <c r="H4" s="37">
+      <c r="H4" s="27">
         <v>3</v>
       </c>
-      <c r="I4" s="32">
+      <c r="I4" s="22">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="31" t="s">
+    <row r="5" spans="1:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="30">
+      <c r="B5" s="20">
         <v>2</v>
       </c>
-      <c r="C5" s="30">
+      <c r="C5" s="20">
         <v>0</v>
       </c>
-      <c r="D5" s="30">
+      <c r="D5" s="20">
         <v>3</v>
       </c>
-      <c r="E5" s="28">
+      <c r="E5" s="18">
         <v>1</v>
       </c>
-      <c r="F5" s="35">
+      <c r="F5" s="25">
         <v>35</v>
       </c>
-      <c r="G5" s="37">
+      <c r="G5" s="27">
         <v>3</v>
       </c>
-      <c r="H5" s="28">
+      <c r="H5" s="18">
         <v>1</v>
       </c>
-      <c r="I5" s="36">
+      <c r="I5" s="26">
         <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="30">
+      <c r="B6" s="20">
         <v>3</v>
       </c>
-      <c r="C6" s="30">
+      <c r="C6" s="20">
         <v>1</v>
       </c>
-      <c r="D6" s="30">
+      <c r="D6" s="20">
         <v>1</v>
       </c>
-      <c r="E6" s="28">
+      <c r="E6" s="18">
         <v>1</v>
       </c>
-      <c r="F6" s="35">
+      <c r="F6" s="25">
         <v>35</v>
       </c>
-      <c r="G6" s="34">
+      <c r="G6" s="24">
         <v>2</v>
       </c>
-      <c r="H6" s="33">
+      <c r="H6" s="23">
         <v>18</v>
       </c>
-      <c r="I6" s="32">
+      <c r="I6" s="22">
         <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="30">
+      <c r="B7" s="20">
         <v>3</v>
       </c>
-      <c r="C7" s="30">
+      <c r="C7" s="20">
         <v>1</v>
       </c>
-      <c r="D7" s="30">
+      <c r="D7" s="20">
         <v>2</v>
       </c>
-      <c r="E7" s="28">
+      <c r="E7" s="18">
         <v>1</v>
       </c>
-      <c r="F7" s="29">
+      <c r="F7" s="19">
         <v>51</v>
       </c>
-      <c r="G7" s="28">
+      <c r="G7" s="18">
         <v>1</v>
       </c>
-      <c r="H7" s="27">
+      <c r="H7" s="17">
         <v>4</v>
       </c>
-      <c r="I7" s="26">
+      <c r="I7" s="16">
         <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="24">
+      <c r="B8" s="43"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="41">
         <v>8</v>
       </c>
-      <c r="F8" s="23">
+      <c r="F8" s="44">
         <v>250</v>
       </c>
-      <c r="G8" s="22">
+      <c r="G8" s="45">
         <v>19</v>
       </c>
-      <c r="H8" s="21">
+      <c r="H8" s="46">
         <v>43</v>
       </c>
-      <c r="I8" s="20">
+      <c r="I8" s="43">
         <v>320</v>
       </c>
     </row>

</xml_diff>